<commit_message>
Reversed list access change, moved to nullables instead of Unknown enum
</commit_message>
<xml_diff>
--- a/documentation/zugferd233de/Dokumentation/4. EN16931+FacturX code lists values v15 - used from 2025-05-15.xlsx
+++ b/documentation/zugferd233de/Dokumentation/4. EN16931+FacturX code lists values v15 - used from 2025-05-15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrille/Documents/_Cyrille_Boulot/ADMAREL_2025/_FNFE_2025/_Factur-x/_Factur-X_V1.07-2024/_Factur-X 1.07.3 - 2025 05 15 VF/_Check xsd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\ZUGFeRD-csharp\documentation\zugferd233de\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE3E6F-9CAB-8243-A45C-2BABE9F3FFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414355FD-0074-4B1A-BB20-6BC4E7769A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21320" yWindow="9800" windowWidth="26400" windowHeight="15620" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42930" yWindow="4080" windowWidth="28800" windowHeight="15345" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -45,6 +45,9 @@
     <sheet name="Filename" sheetId="40" r:id="rId30"/>
     <sheet name="HybridVersion" sheetId="41" r:id="rId31"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Index!$A$7:$H$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33817,21 +33820,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -33853,80 +33841,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Gut" xfId="3" builtinId="26"/>
     <cellStyle name="Nor_x0004_al" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Satisfaisant" xfId="3" builtinId="26"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="97">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -34016,70 +33953,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -34933,6 +34806,18 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -35031,6 +34916,60 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -35279,6 +35218,60 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -35407,46 +35400,46 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table4" displayName="Table4" ref="A1:B20" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table4" displayName="Table4" ref="A1:B20" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:B20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Code" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Description" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Code" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Description" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table13" displayName="Table13" ref="A1:B186" totalsRowShown="0" headerRowDxfId="78" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table13" displayName="Table13" ref="A1:B186" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A1:B186" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Code" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Code name" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Code" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Code name" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table14" displayName="Table14" ref="A1:B179" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table14" displayName="Table14" ref="A1:B179" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A1:B179" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Code" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Code name" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Code" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Code name" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table17" displayName="Table17" ref="A1:A9" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table17" displayName="Table17" ref="A1:A9" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:A9" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Code" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Code" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35467,15 +35460,15 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table15" displayName="Table15" ref="A1:C88" totalsRowShown="0" headerRowDxfId="70" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table15" displayName="Table15" ref="A1:C88" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:C88" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C61">
     <sortCondition ref="A1:A61"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="CODE" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Code name (english)" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Remark" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="CODE" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Code name (english)" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Remark" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35499,45 +35492,45 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table146" displayName="Table146" ref="A1:C120" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table146" displayName="Table146" ref="A1:C120" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:C120" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Code" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Code name" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Description" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Code" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Code name" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Description" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table1469" displayName="Table1469" ref="A1:B484" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table1469" displayName="Table1469" ref="A1:B484" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:B484" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Code" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Code name" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Code" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Code name" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table146917" displayName="Table146917" ref="A1:D316" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table146917" displayName="Table146917" ref="A1:D316" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:D316" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Code list" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Code" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Code name" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="Description" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Code list" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Code" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Code name" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="Description" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35558,111 +35551,111 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table14620" displayName="Table14620" ref="A1:B4" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table14620" displayName="Table14620" ref="A1:B4" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Code" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="Code name" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Code" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="Code name" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table1462021" displayName="Table1462021" ref="A1:B14" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table1462021" displayName="Table1462021" ref="A1:B14" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:B14" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Code" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="Code name" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Code" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="Code name" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Table146202122" displayName="Table146202122" ref="A1:C11" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Table146202122" displayName="Table146202122" ref="A1:C11" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Code" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="Code name" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="Description" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Code" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="Code name" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="Description" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Table14620212223" displayName="Table14620212223" ref="A1:C3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Table14620212223" displayName="Table14620212223" ref="A1:C3" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Code" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="Code name" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="Description" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Code" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="Code name" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="Description" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="Table1462021222325" displayName="Table1462021222325" ref="A1:C5" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="Table1462021222325" displayName="Table1462021222325" ref="A1:C5" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Code" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="Definition" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1700-000004000000}" name="Usage Rule" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Code" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="Definition" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1700-000004000000}" name="Usage Rule" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="Table146202122232526" displayName="Table146202122232526" ref="A1:D8" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="Table146202122232526" displayName="Table146202122232526" ref="A1:D8" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:D8" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Code" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="Definition" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="Usage Rule" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="Comment" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Code" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="Definition" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="Usage Rule" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="Comment" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table14620212223252627" displayName="Table14620212223252627" ref="A1:C4" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table14620212223252627" displayName="Table14620212223252627" ref="A1:C4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:C4" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Code" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="Definition" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="Usage Rule" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Code" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="Definition" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="Usage Rule" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="Table1462021222325262728" displayName="Table1462021222325262728" ref="A1:C6" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="Table1462021222325262728" displayName="Table1462021222325262728" ref="A1:C6" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B179">
     <sortCondition ref="A1:A179"/>
@@ -35677,11 +35670,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table9" displayName="Table9" ref="A1:B236" totalsRowShown="0" headerRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table9" displayName="Table9" ref="A1:B236" totalsRowShown="0" headerRowDxfId="96">
   <autoFilter ref="A1:B236" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Code" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Identifier scheme name" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Code" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Identifier scheme name" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35691,30 +35684,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:C63" totalsRowShown="0">
   <autoFilter ref="A1:C63" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Code" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="EN16931 interpretation" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Code" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="EN16931 interpretation" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1" displayName="Table1" ref="A1:B819" totalsRowShown="0" headerRowDxfId="91" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1" displayName="Table1" ref="A1:B819" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A1:B819" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B818">
     <sortCondition ref="A1:A818"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Code Values" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Code Values" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle23" displayName="Tabelle23" ref="C6:E62" totalsRowShown="0" headerRowDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle23" displayName="Tabelle23" ref="C6:E62" totalsRowShown="0" headerRowDxfId="86">
   <autoFilter ref="C6:E62" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Code"/>
@@ -35732,7 +35725,7 @@
     <sortCondition ref="A1:A402"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Code" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Code" dataDxfId="85"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Code name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -35743,7 +35736,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table11" displayName="Table11" ref="A1:C85" totalsRowShown="0">
   <autoFilter ref="A1:C85" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Code" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Code" dataDxfId="84"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Code name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Usage in EN16931"/>
   </tableColumns>
@@ -35752,12 +35745,12 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table3" displayName="Table3" ref="A1:C10" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table3" displayName="Table3" ref="A1:C10" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:C10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Code" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Name" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Semantic model" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Code" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Name" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Semantic model" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -36062,34 +36055,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="74.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="74.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="15" customWidth="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="58.6640625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="59.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="68.6640625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="4" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="59.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="68.7109375" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="38" t="s">
         <v>8674</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="71" t="s">
         <v>8675</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
@@ -36117,24 +36110,24 @@
       <c r="A4" s="17" t="s">
         <v>1774</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="70" t="s">
         <v>8300</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:8" ht="61.5" customHeight="1">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="70" t="s">
         <v>8301</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-    </row>
-    <row r="6" spans="1:8" ht="16" thickBot="1"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="7" spans="1:8">
       <c r="A7" s="39" t="s">
         <v>133</v>
@@ -36161,7 +36154,7 @@
         <v>8676</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="64">
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="25" t="s">
         <v>0</v>
       </c>
@@ -36192,16 +36185,16 @@
       <c r="B9" s="26" t="s">
         <v>2226</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="62">
         <v>45689</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="63" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="61" t="s">
         <v>10936</v>
       </c>
       <c r="G9" s="28" t="s">
@@ -36211,23 +36204,23 @@
         <v>10870</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="48">
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="62">
         <v>45657</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="63" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="61" t="s">
         <v>10937</v>
       </c>
       <c r="G10" s="28" t="s">
@@ -36244,16 +36237,16 @@
       <c r="B11" s="26">
         <v>1001</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="64" t="s">
         <v>10941</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="63" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="61" t="s">
         <v>10938</v>
       </c>
       <c r="G11" s="28" t="s">
@@ -36270,16 +36263,16 @@
       <c r="B12" s="26">
         <v>1153</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="63" t="s">
         <v>10942</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="63" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="61" t="s">
         <v>10939</v>
       </c>
       <c r="G12" s="28" t="s">
@@ -36296,16 +36289,16 @@
       <c r="B13" s="26" t="s">
         <v>7542</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="63" t="s">
         <v>1604</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="63" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>1771</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="61" t="s">
         <v>10940</v>
       </c>
       <c r="G13" s="28" t="s">
@@ -36314,25 +36307,25 @@
       <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="65" t="s">
         <v>10943</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="66" t="s">
         <v>10944</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="67" t="s">
         <v>1604</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>1771</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="68" t="s">
         <v>10945</v>
       </c>
-      <c r="G14" s="74" t="s">
+      <c r="G14" s="69" t="s">
         <v>10946</v>
       </c>
       <c r="H14" s="31"/>
@@ -36392,7 +36385,7 @@
       <c r="B17" s="26" t="s">
         <v>3613</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="63" t="s">
         <v>10942</v>
       </c>
       <c r="D17" s="26" t="s">
@@ -36416,7 +36409,7 @@
       <c r="B18" s="26" t="s">
         <v>3128</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="63" t="s">
         <v>10942</v>
       </c>
       <c r="D18" s="26" t="s">
@@ -36486,7 +36479,7 @@
       <c r="B21" s="26" t="s">
         <v>3885</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="63" t="s">
         <v>10942</v>
       </c>
       <c r="D21" s="26" t="s">
@@ -36495,7 +36488,7 @@
       <c r="E21" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F21" s="66" t="s">
+      <c r="F21" s="61" t="s">
         <v>10947</v>
       </c>
       <c r="G21" s="28" t="s">
@@ -36510,7 +36503,7 @@
       <c r="B22" s="26" t="s">
         <v>3129</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="63" t="s">
         <v>10942</v>
       </c>
       <c r="D22" s="26" t="s">
@@ -36549,7 +36542,7 @@
       </c>
       <c r="H23" s="31"/>
     </row>
-    <row r="24" spans="1:8" ht="48">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="25" t="s">
         <v>140</v>
       </c>
@@ -36565,7 +36558,7 @@
       <c r="E24" s="29" t="s">
         <v>8624</v>
       </c>
-      <c r="F24" s="66" t="s">
+      <c r="F24" s="61" t="s">
         <v>10948</v>
       </c>
       <c r="G24" s="28" t="s">
@@ -36575,7 +36568,7 @@
         <v>10872</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16">
+    <row r="25" spans="1:8">
       <c r="A25" s="25" t="s">
         <v>130</v>
       </c>
@@ -36601,7 +36594,7 @@
         <v>10873</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16" thickBot="1">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" s="46" t="s">
         <v>131</v>
       </c>
@@ -36754,7 +36747,7 @@
         <v>10686</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="64">
+    <row r="33" spans="1:8" ht="60">
       <c r="A33" s="35" t="s">
         <v>10714</v>
       </c>
@@ -36864,6 +36857,7 @@
       <c r="H37" s="55"/>
     </row>
   </sheetData>
+  <autoFilter ref="A7:H7" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
@@ -36882,23 +36876,23 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A1" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="64"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:4" ht="24.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
@@ -36912,7 +36906,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -36926,7 +36920,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
       <c r="A4" s="1">
         <v>35</v>
       </c>
@@ -36940,7 +36934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
       <c r="A5" s="1">
         <v>432</v>
       </c>
@@ -36971,9 +36965,9 @@
       <selection activeCell="A402" sqref="A2:A402"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -41283,7 +41277,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A402">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -41300,10 +41294,10 @@
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42021,13 +42015,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -42038,7 +42032,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>78</v>
       </c>
@@ -42049,7 +42043,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16">
+    <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
         <v>80</v>
       </c>
@@ -42060,7 +42054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16">
+    <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
         <v>82</v>
       </c>
@@ -42071,7 +42065,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16">
+    <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
         <v>84</v>
       </c>
@@ -42082,7 +42076,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32">
+    <row r="6" spans="1:3" ht="45">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -42093,7 +42087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="9" t="s">
         <v>90</v>
       </c>
@@ -42104,7 +42098,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="9" t="s">
         <v>92</v>
       </c>
@@ -42115,7 +42109,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" s="9" t="s">
         <v>95</v>
       </c>
@@ -42126,7 +42120,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="9" t="s">
         <v>98</v>
       </c>
@@ -42151,12 +42145,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="48.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -42164,7 +42158,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16">
+    <row r="2" spans="1:2">
       <c r="A2" s="9">
         <v>41</v>
       </c>
@@ -42172,7 +42166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16">
+    <row r="3" spans="1:2">
       <c r="A3" s="9">
         <v>42</v>
       </c>
@@ -42180,7 +42174,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
+    <row r="4" spans="1:2">
       <c r="A4" s="9">
         <v>60</v>
       </c>
@@ -42188,7 +42182,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16">
+    <row r="5" spans="1:2">
       <c r="A5" s="9">
         <v>62</v>
       </c>
@@ -42196,7 +42190,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16">
+    <row r="6" spans="1:2">
       <c r="A6" s="9">
         <v>63</v>
       </c>
@@ -42204,7 +42198,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16">
+    <row r="7" spans="1:2">
       <c r="A7" s="9">
         <v>64</v>
       </c>
@@ -42212,7 +42206,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16">
+    <row r="8" spans="1:2">
       <c r="A8" s="9">
         <v>65</v>
       </c>
@@ -42220,7 +42214,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16">
+    <row r="9" spans="1:2">
       <c r="A9" s="9">
         <v>66</v>
       </c>
@@ -42228,7 +42222,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16">
+    <row r="10" spans="1:2">
       <c r="A10" s="9">
         <v>67</v>
       </c>
@@ -42236,7 +42230,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16">
+    <row r="11" spans="1:2">
       <c r="A11" s="9">
         <v>68</v>
       </c>
@@ -42244,7 +42238,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16">
+    <row r="12" spans="1:2">
       <c r="A12" s="9">
         <v>70</v>
       </c>
@@ -42252,7 +42246,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16">
+    <row r="13" spans="1:2">
       <c r="A13" s="9">
         <v>71</v>
       </c>
@@ -42260,7 +42254,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16">
+    <row r="14" spans="1:2">
       <c r="A14" s="9">
         <v>88</v>
       </c>
@@ -42268,7 +42262,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16">
+    <row r="15" spans="1:2">
       <c r="A15" s="9">
         <v>95</v>
       </c>
@@ -42276,7 +42270,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16">
+    <row r="16" spans="1:2">
       <c r="A16" s="9">
         <v>100</v>
       </c>
@@ -42284,7 +42278,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16">
+    <row r="17" spans="1:2">
       <c r="A17" s="9">
         <v>102</v>
       </c>
@@ -42292,7 +42286,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16">
+    <row r="18" spans="1:2">
       <c r="A18" s="9">
         <v>103</v>
       </c>
@@ -42300,7 +42294,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16">
+    <row r="19" spans="1:2">
       <c r="A19" s="9">
         <v>104</v>
       </c>
@@ -42308,7 +42302,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16">
+    <row r="20" spans="1:2">
       <c r="A20" s="9">
         <v>105</v>
       </c>
@@ -42332,10 +42326,10 @@
       <selection activeCell="A2" sqref="A2:B186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -43843,10 +43837,10 @@
       <selection activeCell="A2" sqref="A2:B179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -45829,52 +45823,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="84.1640625" customWidth="1"/>
+    <col min="1" max="1" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16">
+    <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16">
+    <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16">
+    <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16">
+    <row r="4" spans="1:1">
       <c r="A4" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16">
+    <row r="5" spans="1:1">
       <c r="A5" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16">
+    <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="16">
+    <row r="7" spans="1:1">
       <c r="A7" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="16">
+    <row r="8" spans="1:1">
       <c r="A8" s="54" t="s">
         <v>10711</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="16">
+    <row r="9" spans="1:1">
       <c r="A9" s="54" t="s">
         <v>10712</v>
       </c>
@@ -45895,9 +45889,9 @@
       <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="154.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="154.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -46196,7 +46190,7 @@
         <v>8420</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16">
+    <row r="38" spans="1:2">
       <c r="A38" s="12" t="s">
         <v>8411</v>
       </c>
@@ -46204,7 +46198,7 @@
         <v>8412</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16">
+    <row r="39" spans="1:2">
       <c r="A39" s="12" t="s">
         <v>8418</v>
       </c>
@@ -46212,7 +46206,7 @@
         <v>8419</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16">
+    <row r="40" spans="1:2">
       <c r="A40" s="12" t="s">
         <v>8425</v>
       </c>
@@ -46220,7 +46214,7 @@
         <v>8429</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16">
+    <row r="41" spans="1:2">
       <c r="A41" s="12" t="s">
         <v>8426</v>
       </c>
@@ -46228,7 +46222,7 @@
         <v>8430</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16">
+    <row r="42" spans="1:2">
       <c r="A42" s="12" t="s">
         <v>8427</v>
       </c>
@@ -46236,7 +46230,7 @@
         <v>8431</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16">
+    <row r="43" spans="1:2">
       <c r="A43" s="12" t="s">
         <v>8428</v>
       </c>
@@ -46260,7 +46254,7 @@
         <v>8542</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16">
+    <row r="46" spans="1:2">
       <c r="A46" s="12" t="s">
         <v>8594</v>
       </c>
@@ -46268,7 +46262,7 @@
         <v>8598</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16">
+    <row r="47" spans="1:2">
       <c r="A47" s="12" t="s">
         <v>8595</v>
       </c>
@@ -46701,12 +46695,12 @@
       <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="78.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="15"/>
+    <col min="1" max="1" width="23.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="78.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -46720,7 +46714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48">
+    <row r="2" spans="1:3" ht="60">
       <c r="A2" s="15" t="s">
         <v>8422</v>
       </c>
@@ -47123,7 +47117,7 @@
         <v>4168</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="16">
+    <row r="52" spans="1:3">
       <c r="A52" s="60" t="s">
         <v>10968</v>
       </c>
@@ -47257,7 +47251,7 @@
         <v>8635</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16">
+    <row r="65" spans="1:3">
       <c r="A65" s="22" t="s">
         <v>10970</v>
       </c>
@@ -47268,7 +47262,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16">
+    <row r="66" spans="1:3">
       <c r="A66" s="22" t="s">
         <v>10973</v>
       </c>
@@ -47279,7 +47273,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16">
+    <row r="67" spans="1:3">
       <c r="A67" s="22" t="s">
         <v>10975</v>
       </c>
@@ -47290,7 +47284,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16">
+    <row r="68" spans="1:3">
       <c r="A68" s="22" t="s">
         <v>10977</v>
       </c>
@@ -47301,7 +47295,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="16">
+    <row r="69" spans="1:3">
       <c r="A69" s="22" t="s">
         <v>10979</v>
       </c>
@@ -47312,7 +47306,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="16">
+    <row r="70" spans="1:3">
       <c r="A70" s="22" t="s">
         <v>10981</v>
       </c>
@@ -47323,7 +47317,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16">
+    <row r="71" spans="1:3">
       <c r="A71" s="22" t="s">
         <v>10983</v>
       </c>
@@ -47334,7 +47328,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="16">
+    <row r="72" spans="1:3">
       <c r="A72" s="22" t="s">
         <v>10985</v>
       </c>
@@ -47345,7 +47339,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16">
+    <row r="73" spans="1:3">
       <c r="A73" s="22" t="s">
         <v>10987</v>
       </c>
@@ -47356,7 +47350,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16">
+    <row r="74" spans="1:3">
       <c r="A74" s="22" t="s">
         <v>10989</v>
       </c>
@@ -47367,7 +47361,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16">
+    <row r="75" spans="1:3">
       <c r="A75" s="22" t="s">
         <v>10991</v>
       </c>
@@ -47378,7 +47372,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16">
+    <row r="76" spans="1:3">
       <c r="A76" s="22" t="s">
         <v>10993</v>
       </c>
@@ -47389,7 +47383,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16">
+    <row r="77" spans="1:3">
       <c r="A77" s="22" t="s">
         <v>10995</v>
       </c>
@@ -47400,7 +47394,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16">
+    <row r="78" spans="1:3">
       <c r="A78" s="22" t="s">
         <v>10997</v>
       </c>
@@ -47411,7 +47405,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16">
+    <row r="79" spans="1:3">
       <c r="A79" s="22" t="s">
         <v>10999</v>
       </c>
@@ -47422,7 +47416,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16">
+    <row r="80" spans="1:3">
       <c r="A80" s="22" t="s">
         <v>11001</v>
       </c>
@@ -47433,7 +47427,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16">
+    <row r="81" spans="1:3">
       <c r="A81" s="22" t="s">
         <v>11003</v>
       </c>
@@ -47444,7 +47438,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16">
+    <row r="82" spans="1:3">
       <c r="A82" s="22" t="s">
         <v>11005</v>
       </c>
@@ -47455,7 +47449,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16">
+    <row r="83" spans="1:3">
       <c r="A83" s="22" t="s">
         <v>11007</v>
       </c>
@@ -47466,7 +47460,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16">
+    <row r="84" spans="1:3">
       <c r="A84" s="22" t="s">
         <v>11009</v>
       </c>
@@ -47477,7 +47471,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16">
+    <row r="85" spans="1:3">
       <c r="A85" s="22" t="s">
         <v>11011</v>
       </c>
@@ -47488,7 +47482,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16">
+    <row r="86" spans="1:3" ht="30">
       <c r="A86" s="22" t="s">
         <v>11013</v>
       </c>
@@ -47499,7 +47493,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16">
+    <row r="87" spans="1:3">
       <c r="A87" s="22" t="s">
         <v>11015</v>
       </c>
@@ -47510,7 +47504,7 @@
         <v>10972</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16">
+    <row r="88" spans="1:3">
       <c r="A88" s="22" t="s">
         <v>11017</v>
       </c>
@@ -47537,10 +47531,10 @@
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -49575,12 +49569,12 @@
       <selection activeCell="B2064" sqref="B2064"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -73381,18 +73375,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2134">
-    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B2134">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2115:B2134">
-    <cfRule type="duplicateValues" dxfId="10" priority="8" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="8" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2135:B2163">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="3" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -73409,10 +73403,10 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -74930,10 +74924,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -78824,10 +78818,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="241" bestFit="1" customWidth="1"/>
   </cols>
@@ -82972,7 +82966,7 @@
         <v>10608</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="64">
+    <row r="297" spans="1:4" ht="60">
       <c r="A297" s="15" t="s">
         <v>10593</v>
       </c>
@@ -82986,7 +82980,7 @@
         <v>10612</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="64">
+    <row r="298" spans="1:4" ht="60">
       <c r="A298" s="15" t="s">
         <v>10593</v>
       </c>
@@ -83038,7 +83032,7 @@
         <v>10615</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="48">
+    <row r="302" spans="1:4" ht="45">
       <c r="A302" s="15" t="s">
         <v>10593</v>
       </c>
@@ -83178,7 +83172,7 @@
         <v>10639</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="48">
+    <row r="313" spans="1:4" ht="45">
       <c r="A313" s="15" t="s">
         <v>10593</v>
       </c>
@@ -83246,10 +83240,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -83480,10 +83474,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -83764,15 +83758,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -83783,7 +83777,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="64">
+    <row r="2" spans="1:3" ht="75">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -83794,7 +83788,7 @@
         <v>10690</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16">
+    <row r="3" spans="1:3">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -83805,7 +83799,7 @@
         <v>10692</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16">
+    <row r="4" spans="1:3">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -83816,7 +83810,7 @@
         <v>10694</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16">
+    <row r="5" spans="1:3">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -83827,7 +83821,7 @@
         <v>10696</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16">
+    <row r="6" spans="1:3">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -83838,7 +83832,7 @@
         <v>10698</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="112">
+    <row r="7" spans="1:3" ht="105">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -83849,7 +83843,7 @@
         <v>10700</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="144">
+    <row r="8" spans="1:3" ht="165">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -83860,7 +83854,7 @@
         <v>10702</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="64">
+    <row r="9" spans="1:3" ht="60">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -83871,7 +83865,7 @@
         <v>10704</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16">
+    <row r="10" spans="1:3">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -83882,7 +83876,7 @@
         <v>10706</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16">
+    <row r="11" spans="1:3">
       <c r="A11" s="15">
         <v>9</v>
       </c>
@@ -83909,15 +83903,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -83928,7 +83922,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16">
+    <row r="2" spans="1:3">
       <c r="A2" s="15">
         <v>102</v>
       </c>
@@ -83939,7 +83933,7 @@
         <v>10716</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="32">
+    <row r="3" spans="1:3" ht="60">
       <c r="A3" s="15">
         <v>205</v>
       </c>
@@ -83964,15 +83958,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -83983,7 +83977,7 @@
         <v>10885</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16">
+    <row r="2" spans="1:3">
       <c r="A2" s="15" t="s">
         <v>10886</v>
       </c>
@@ -83994,7 +83988,7 @@
         <v>10888</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16">
+    <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
         <v>10889</v>
       </c>
@@ -84005,7 +83999,7 @@
         <v>10891</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16">
+    <row r="4" spans="1:3">
       <c r="A4" s="15" t="s">
         <v>10892</v>
       </c>
@@ -84016,7 +84010,7 @@
         <v>10891</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16">
+    <row r="5" spans="1:3">
       <c r="A5" s="15" t="s">
         <v>10894</v>
       </c>
@@ -84042,16 +84036,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="15" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="4" width="36.140625" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:4">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -84065,7 +84059,7 @@
         <v>3262</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16">
+    <row r="2" spans="1:4">
       <c r="A2" s="15" t="s">
         <v>10896</v>
       </c>
@@ -84079,7 +84073,7 @@
         <v>10899</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16">
+    <row r="3" spans="1:4">
       <c r="A3" s="15" t="s">
         <v>10900</v>
       </c>
@@ -84093,7 +84087,7 @@
         <v>10899</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="15" t="s">
         <v>10902</v>
       </c>
@@ -84105,7 +84099,7 @@
       </c>
       <c r="D4" s="33"/>
     </row>
-    <row r="5" spans="1:4" ht="16">
+    <row r="5" spans="1:4">
       <c r="A5" s="15" t="s">
         <v>10905</v>
       </c>
@@ -84117,7 +84111,7 @@
       </c>
       <c r="D5" s="33"/>
     </row>
-    <row r="6" spans="1:4" ht="16">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="15" t="s">
         <v>10907</v>
       </c>
@@ -84129,7 +84123,7 @@
       </c>
       <c r="D6" s="33"/>
     </row>
-    <row r="7" spans="1:4" ht="32">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="15" t="s">
         <v>10910</v>
       </c>
@@ -84141,7 +84135,7 @@
       </c>
       <c r="D7" s="33"/>
     </row>
-    <row r="8" spans="1:4" ht="16">
+    <row r="8" spans="1:4">
       <c r="A8" s="15" t="s">
         <v>10912</v>
       </c>
@@ -84172,10 +84166,10 @@
       <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -85612,7 +85606,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B179">
-    <cfRule type="duplicateValues" dxfId="16" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -85629,15 +85623,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -85648,7 +85642,7 @@
         <v>10885</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16">
+    <row r="2" spans="1:3">
       <c r="A2" s="15" t="s">
         <v>10916</v>
       </c>
@@ -85659,7 +85653,7 @@
         <v>10918</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16">
+    <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
         <v>10919</v>
       </c>
@@ -85694,15 +85688,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="62" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -85713,7 +85707,7 @@
         <v>10885</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" thickBot="1">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" s="57" t="s">
         <v>10924</v>
       </c>
@@ -85724,7 +85718,7 @@
         <v>10926</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="33" thickBot="1">
+    <row r="3" spans="1:3" ht="30.75" thickBot="1">
       <c r="A3" s="57" t="s">
         <v>10927</v>
       </c>
@@ -85735,7 +85729,7 @@
         <v>10929</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="33" thickBot="1">
+    <row r="4" spans="1:3" ht="30.75" thickBot="1">
       <c r="A4" s="57" t="s">
         <v>10930</v>
       </c>
@@ -85746,7 +85740,7 @@
         <v>10929</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="33" thickBot="1">
+    <row r="5" spans="1:3" ht="30.75" thickBot="1">
       <c r="A5" s="57" t="s">
         <v>10932</v>
       </c>
@@ -85757,7 +85751,7 @@
         <v>10929</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="33" thickBot="1">
+    <row r="6" spans="1:3" ht="30.75" thickBot="1">
       <c r="A6" s="57" t="s">
         <v>10934</v>
       </c>
@@ -85785,11 +85779,11 @@
       <selection activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="154.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="11"/>
+    <col min="1" max="1" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="154.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -87416,7 +87410,7 @@
         <v>8417</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="16">
+    <row r="204" spans="1:2">
       <c r="A204" s="12" t="s">
         <v>8411</v>
       </c>
@@ -87488,7 +87482,7 @@
         <v>8542</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="16">
+    <row r="213" spans="1:2">
       <c r="A213" s="12" t="s">
         <v>8594</v>
       </c>
@@ -87700,11 +87694,11 @@
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -88416,13 +88410,13 @@
       <selection activeCell="H622" sqref="H622"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>1770</v>
       </c>
@@ -94976,7 +94970,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A816:A818">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -94993,33 +94987,33 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:4" ht="15.95" customHeight="1" thickBot="1">
+      <c r="A1" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="72" t="s">
         <v>7541</v>
       </c>
-      <c r="D1" s="64"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A2" s="63" t="s">
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.95" customHeight="1" thickBot="1">
+      <c r="A2" s="72" t="s">
         <v>8623</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="63" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="72" t="s">
         <v>8621</v>
       </c>
-      <c r="D2" s="64"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+      <c r="D2" s="73"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -95033,7 +95027,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>143</v>
       </c>
@@ -95066,12 +95060,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -95079,7 +95073,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>1501</v>
       </c>
@@ -95100,24 +95094,24 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
     <col min="5" max="5" width="163" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="72" t="s">
         <v>7541</v>
       </c>
-      <c r="D1" s="64"/>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1">
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -95131,7 +95125,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>143</v>
       </c>
@@ -95146,11 +95140,11 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="74" t="s">
         <v>10869</v>
       </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="30" t="s">

</xml_diff>